<commit_message>
Janjan Manzanal name added as part of testing team.
</commit_message>
<xml_diff>
--- a/updatetestcases/UpdateTestingDocument20Oct2015.xlsx
+++ b/updatetestcases/UpdateTestingDocument20Oct2015.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="409">
   <si>
     <t>Test Condition</t>
   </si>
@@ -2718,6 +2718,28 @@
   </si>
   <si>
     <t>Sytax Errors Must be addressed and resolved by Gladys (parser)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tester:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Venus D. Retuya/Wenceslao Navallo/J.Manzanal</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3038,6 +3060,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3047,11 +3074,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3335,7 +3357,7 @@
   <dimension ref="B1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3350,42 +3372,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="67"/>
+      <c r="C2" s="70"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="B4" s="70" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="58" t="s">
@@ -3570,18 +3592,18 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="66" t="s">
         <v>385</v>
       </c>
-      <c r="C18" s="70">
+      <c r="C18" s="67">
         <f>C17/E17</f>
         <v>0.93867924528301883</v>
       </c>
-      <c r="D18" s="71">
+      <c r="D18" s="68">
         <f>D17/E17</f>
         <v>6.1320754716981132E-2</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="67">
         <f>SUM(C18:D18)</f>
         <v>1</v>
       </c>
@@ -3641,27 +3663,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -3671,10 +3693,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -3684,10 +3706,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -4356,27 +4378,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -4386,10 +4408,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -4399,10 +4421,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -5492,27 +5514,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -5522,10 +5544,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -5535,10 +5557,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -6149,27 +6171,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -6179,10 +6201,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -6192,10 +6214,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -6840,27 +6862,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -6870,10 +6892,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -6883,10 +6905,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -7173,27 +7195,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -7203,10 +7225,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -7216,10 +7238,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -7444,27 +7466,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -7474,10 +7496,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -7487,10 +7509,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -7702,27 +7724,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -7732,10 +7754,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -7745,10 +7767,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
@@ -7960,27 +7982,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="70"/>
       <c r="E2" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -7990,10 +8012,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
@@ -8003,10 +8025,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="7" t="s">
         <v>49</v>
       </c>

</xml_diff>